<commit_message>
búnað setja inn user stories og prioritysa það að minni bestu vitund
</commit_message>
<xml_diff>
--- a/Progress_Tracking_sheet.xlsx
+++ b/Progress_Tracking_sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\OneDrive\Desktop\háskóli íslands\Þróun Hugbúnaðar\Throun_Hugbunadar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>User Story ID</t>
   </si>
@@ -459,7 +459,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,8 +517,8 @@
       <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
+      <c r="D4" s="3">
+        <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>2</v>
@@ -539,50 +539,80 @@
       <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C10" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C12" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C13" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="C14" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C15" s="7" t="s">
         <v>22</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>